<commit_message>
New Excel, with the results in blocks, and new #sample
</commit_message>
<xml_diff>
--- a/doc/Results/Resultados por Bloque.xlsx
+++ b/doc/Results/Resultados por Bloque.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BE7252-217F-411A-AA34-AA1CE927B105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA8495C-7772-4192-84D1-6FB05663BF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4536" yWindow="4608" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PC por Bloque" sheetId="1" r:id="rId1"/>
@@ -912,7 +912,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -922,6 +922,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="L114" sqref="L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11143,10 +11144,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B62AD6E-4C46-4D86-966D-E6532A5E9179}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q241"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K222" sqref="K222:L222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11246,7 +11248,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11292,7 +11294,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -11332,7 +11334,7 @@
         <v>16.986207054506629</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -11372,7 +11374,7 @@
         <v>7.3758719999983749E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -11412,7 +11414,7 @@
         <v>1.8321870933330639E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -11452,7 +11454,7 @@
         <v>0.20845619200000376</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -11492,7 +11494,7 @@
         <v>2.0517368017066735</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -11532,7 +11534,7 @@
         <v>1.6562783999999681E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -11572,7 +11574,7 @@
         <v>2.590160383999876E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -11652,7 +11654,7 @@
         <v>3.7748659199999479E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -11692,7 +11694,7 @@
         <v>3.5345793279998781E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -11732,7 +11734,7 @@
         <v>16.37955680256</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -11772,7 +11774,7 @@
         <v>9.373503999999469E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -11812,7 +11814,7 @@
         <v>0.28449865173333111</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -11852,7 +11854,7 @@
         <v>0.19641917866667591</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -11892,7 +11894,7 @@
         <v>9.9765873446399898</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -11932,7 +11934,7 @@
         <v>6.4528928426666188E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -11972,7 +11974,7 @@
         <v>4.1035971199998883E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -12052,7 +12054,7 @@
         <v>3.7511577599999221E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -12092,7 +12094,7 @@
         <v>2.8443206400002054E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -12132,7 +12134,7 @@
         <v>15.166256298666633</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -12172,7 +12174,7 @@
         <v>1.9612648533332663E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -12212,7 +12214,7 @@
         <v>0.47650181973334793</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -12252,7 +12254,7 @@
         <v>0.6005975001599918</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -12292,7 +12294,7 @@
         <v>0.17672062464000132</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -12332,7 +12334,7 @@
         <v>4.4105665706666464E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -12372,7 +12374,7 @@
         <v>1.8748544639999708E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -12452,7 +12454,7 @@
         <v>3.9961420799999196E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -12492,7 +12494,7 @@
         <v>9.5509859200001046E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -12532,7 +12534,7 @@
         <v>16.986207054506629</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -12572,7 +12574,7 @@
         <v>7.2918690133332312E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -12612,7 +12614,7 @@
         <v>0.17876245333332871</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -12652,7 +12654,7 @@
         <v>0.26686124416000223</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -12692,7 +12694,7 @@
         <v>0.13414794026666507</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -12732,7 +12734,7 @@
         <v>4.2937819306666035E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -12772,7 +12774,7 @@
         <v>3.3431139839997813E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -12852,7 +12854,7 @@
         <v>1.706428475733329</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -12892,7 +12894,7 @@
         <v>0.50266106687998235</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -12932,7 +12934,7 @@
         <v>15.166256298666633</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -12972,7 +12974,7 @@
         <v>0.37864858453334704</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -13012,7 +13014,7 @@
         <v>4.0152403200001602E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -13052,7 +13054,7 @@
         <v>1.0833592985600129</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -13092,7 +13094,7 @@
         <v>0.48540233130666638</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -13132,7 +13134,7 @@
         <v>0.84932683136000098</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -13172,7 +13174,7 @@
         <v>9.3001038293332686E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -13252,7 +13254,7 @@
         <v>5.2550622058666079</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -13292,7 +13294,7 @@
         <v>2.8429499571199632</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -13332,7 +13334,7 @@
         <v>16.37955680256</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -13372,7 +13374,7 @@
         <v>1.1921867775999651</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -13412,7 +13414,7 @@
         <v>3.7323909951999839</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -13452,7 +13454,7 @@
         <v>0.48003799424000254</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -13492,7 +13494,7 @@
         <v>11.426454308266674</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -13532,7 +13534,7 @@
         <v>7.4903916326399758</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -13572,7 +13574,7 @@
         <v>0.75477861610665486</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -13652,7 +13654,7 @@
         <v>2.6430588501333458</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -13692,7 +13694,7 @@
         <v>2.2230616979200302</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -13732,7 +13734,7 @@
         <v>16.379556802559971</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -13772,7 +13774,7 @@
         <v>1.3373890133332112E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -13812,7 +13814,7 @@
         <v>0.90339577813334371</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -13852,7 +13854,7 @@
         <v>0.19555939199999553</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -13892,7 +13894,7 @@
         <v>0.23960710442666575</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -13932,7 +13934,7 @@
         <v>0.27718014762666565</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -13972,7 +13974,7 @@
         <v>0.1698130619733326</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -14052,7 +14054,7 @@
         <v>2.2185181461333316</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -14092,7 +14094,7 @@
         <v>0.75973479231999985</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -14132,7 +14134,7 @@
         <v>16.986207054506629</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -14172,7 +14174,7 @@
         <v>1.8196942101333275</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -14212,7 +14214,7 @@
         <v>0.88142182613335673</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -14252,7 +14254,7 @@
         <v>4.4073469439998771E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -14292,7 +14294,7 @@
         <v>0.29514288384000054</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -14332,7 +14334,7 @@
         <v>0.39536649599999679</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -14372,7 +14374,7 @@
         <v>6.9518276551109953E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -14452,7 +14454,7 @@
         <v>4.3201535999992189E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -14492,7 +14494,7 @@
         <v>0.34362036351999775</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -14532,7 +14534,7 @@
         <v>29.101338043306605</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -14572,7 +14574,7 @@
         <v>2.09495253333348E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -14612,7 +14614,7 @@
         <v>5.9467967999992551E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -14652,7 +14654,7 @@
         <v>0.12123094442667073</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -14692,7 +14694,7 @@
         <v>4.6350477226666319E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -14732,7 +14734,7 @@
         <v>3.613226026666759E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -14772,7 +14774,7 @@
         <v>3.8852405759998765E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -14852,7 +14854,7 @@
         <v>1.2486297600000532E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -14892,7 +14894,7 @@
         <v>7.972088320000334E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -14932,7 +14934,7 @@
         <v>35.157712495359959</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -14972,7 +14974,7 @@
         <v>8.62567253333308E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>109</v>
       </c>
@@ -15012,7 +15014,7 @@
         <v>8.34907733333138E-4</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -15052,7 +15054,7 @@
         <v>0.1771697625599975</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -15092,7 +15094,7 @@
         <v>5.1719351040000035E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -15132,7 +15134,7 @@
         <v>2.7037107626667972E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>113</v>
       </c>
@@ -15172,7 +15174,7 @@
         <v>3.0896708266668141E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>114</v>
       </c>
@@ -15252,7 +15254,7 @@
         <v>1.0115481599999539E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>116</v>
       </c>
@@ -15292,7 +15294,7 @@
         <v>5.3905331199998456E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>117</v>
       </c>
@@ -15332,7 +15334,7 @@
         <v>10.919704535039987</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -15372,7 +15374,7 @@
         <v>1.7307688533333671E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>119</v>
       </c>
@@ -15412,7 +15414,7 @@
         <v>1.9412885333322477E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>120</v>
       </c>
@@ -15452,7 +15454,7 @@
         <v>8.4552225706668191E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>121</v>
       </c>
@@ -15492,7 +15494,7 @@
         <v>8.6953628159995799E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -15532,7 +15534,7 @@
         <v>1.1156006399999212E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>123</v>
       </c>
@@ -15572,7 +15574,7 @@
         <v>1.423082303999936E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>124</v>
       </c>
@@ -15652,7 +15654,7 @@
         <v>1.2618009599999737E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -15692,7 +15694,7 @@
         <v>3.3391187199997116E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>127</v>
       </c>
@@ -15732,7 +15734,7 @@
         <v>24.242178986666655</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -15772,7 +15774,7 @@
         <v>7.23040341333335E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>129</v>
       </c>
@@ -15812,7 +15814,7 @@
         <v>6.1516821333333655E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>130</v>
       </c>
@@ -15852,7 +15854,7 @@
         <v>0.4438233408000084</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>131</v>
       </c>
@@ -15892,7 +15894,7 @@
         <v>2.905574330026667</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>132</v>
       </c>
@@ -15932,7 +15934,7 @@
         <v>1.2796845226667915E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>133</v>
       </c>
@@ -15972,7 +15974,7 @@
         <v>1.0842531839998617E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>134</v>
       </c>
@@ -16052,7 +16054,7 @@
         <v>0.22678172160000282</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -16092,7 +16094,7 @@
         <v>2.3269339520001164E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -16132,7 +16134,7 @@
         <v>7.878708170666636</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -16172,7 +16174,7 @@
         <v>1.6185941333329771E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -16212,7 +16214,7 @@
         <v>1.2651669333336689E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -16252,7 +16254,7 @@
         <v>0.10417365503999958</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -16292,7 +16294,7 @@
         <v>0.12033603455999954</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -16332,7 +16334,7 @@
         <v>0.13361406762666728</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -16372,7 +16374,7 @@
         <v>3.7164321351112937E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -16452,7 +16454,7 @@
         <v>5.4792192000009928E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -16492,7 +16494,7 @@
         <v>9.1622159999999161E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -16532,7 +16534,7 @@
         <v>4.2423813226666693</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -16572,7 +16574,7 @@
         <v>2.8432962133333288E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -16612,7 +16614,7 @@
         <v>9.7320533333505245E-5</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -16652,7 +16654,7 @@
         <v>0.25559035562666876</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -16692,7 +16694,7 @@
         <v>7.3048938666669186E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -16732,7 +16734,7 @@
         <v>3.2110214826666886E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -16772,7 +16774,7 @@
         <v>0.28313599352889218</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -16852,7 +16854,7 @@
         <v>1.1373331199999786E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -16892,7 +16894,7 @@
         <v>2.5969215999999882E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -16932,7 +16934,7 @@
         <v>7.878708170666636</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -16972,7 +16974,7 @@
         <v>3.0323029333326657E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -17012,7 +17014,7 @@
         <v>1.3384134400000535E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -17052,7 +17054,7 @@
         <v>0.27805647146666546</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -17092,7 +17094,7 @@
         <v>9.1107824639999002E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -17132,7 +17134,7 @@
         <v>3.9295543466666839E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -17172,7 +17174,7 @@
         <v>1.1746076159999968E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -17252,7 +17254,7 @@
         <v>9.4605802666673372E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -17292,7 +17294,7 @@
         <v>5.3155450880001016E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>168</v>
       </c>
@@ -17332,7 +17334,7 @@
         <v>9.0908171200000005</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>169</v>
       </c>
@@ -17372,7 +17374,7 @@
         <v>7.9341845333340093E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -17412,7 +17414,7 @@
         <v>1.3266325333340077E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -17452,7 +17454,7 @@
         <v>4.4348454826666904E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -17492,7 +17494,7 @@
         <v>7.7405971626666056E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -17532,7 +17534,7 @@
         <v>1.4024693760000647E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -17572,7 +17574,7 @@
         <v>5.195379840000171E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -17638,21 +17640,21 @@
         <v>2.4155946190476341E-2</v>
       </c>
       <c r="I162">
-        <v>0.1554218330559653</v>
+        <v>0.105421833055965</v>
       </c>
       <c r="J162">
         <v>15.088285714285711</v>
       </c>
       <c r="K162" s="3">
         <f t="shared" si="4"/>
-        <v>1.714064654220921</v>
+        <v>1.1626412729242535</v>
       </c>
       <c r="L162" s="3">
-        <f t="shared" si="5"/>
-        <v>37.11899315413357</v>
-      </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+        <f>(($Q$2*I162)/($Q$3))^2</f>
+        <v>17.077852599421625</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>178</v>
       </c>
@@ -17692,7 +17694,7 @@
         <v>2.1270017216000343</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>179</v>
       </c>
@@ -17732,7 +17734,7 @@
         <v>13.346305542826693</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>180</v>
       </c>
@@ -17772,7 +17774,7 @@
         <v>2.3019225749332959</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>181</v>
       </c>
@@ -17812,7 +17814,7 @@
         <v>0.19580379093336947</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>182</v>
       </c>
@@ -17852,7 +17854,7 @@
         <v>0.20593712682666238</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>183</v>
       </c>
@@ -17892,7 +17894,7 @@
         <v>0.53273523370666875</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>184</v>
       </c>
@@ -17932,7 +17934,7 @@
         <v>0.52319123583999361</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>185</v>
       </c>
@@ -17972,7 +17974,7 @@
         <v>0.17018885582222479</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>186</v>
       </c>
@@ -18052,7 +18054,7 @@
         <v>17.204976588800054</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>188</v>
       </c>
@@ -18092,7 +18094,7 @@
         <v>2.3999827443199417</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>189</v>
       </c>
@@ -18132,7 +18134,7 @@
         <v>10.91970453504001</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -18172,7 +18174,7 @@
         <v>5.4109755541335183</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>191</v>
       </c>
@@ -18212,7 +18214,7 @@
         <v>4.4338671552000744</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>192</v>
       </c>
@@ -18252,7 +18254,7 @@
         <v>0.39964757504000337</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>193</v>
       </c>
@@ -18292,7 +18294,7 @@
         <v>0.34298434090666574</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>194</v>
       </c>
@@ -18332,7 +18334,7 @@
         <v>0.2250185369600001</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>195</v>
       </c>
@@ -18372,7 +18374,7 @@
         <v>0.35645079530666507</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>196</v>
       </c>
@@ -18412,7 +18414,7 @@
         <v>7.0708593750044759</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>197</v>
       </c>
@@ -18443,16 +18445,16 @@
       <c r="J182">
         <v>9.4238571428571429</v>
       </c>
-      <c r="K182">
+      <c r="K182" s="3">
         <f t="shared" si="4"/>
         <v>1.6628470360234275</v>
       </c>
-      <c r="L182">
+      <c r="L182" s="3">
         <f t="shared" si="5"/>
         <v>13.62769623040003</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>198</v>
       </c>
@@ -18492,7 +18494,7 @@
         <v>3.1788056787199741</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>199</v>
       </c>
@@ -18532,7 +18534,7 @@
         <v>16.363470816000007</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>200</v>
       </c>
@@ -18572,7 +18574,7 @@
         <v>1.8143467029333538</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>201</v>
       </c>
@@ -18612,7 +18614,7 @@
         <v>4.8988129811413241</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>202</v>
       </c>
@@ -18652,7 +18654,7 @@
         <v>0.12729233066666437</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>203</v>
       </c>
@@ -18692,7 +18694,7 @@
         <v>0.1247707775999987</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>204</v>
       </c>
@@ -18732,7 +18734,7 @@
         <v>0.46064047530666952</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>205</v>
       </c>
@@ -18772,7 +18774,7 @@
         <v>0.20977201927111208</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>206</v>
       </c>
@@ -18852,7 +18854,7 @@
         <v>18.989052947199966</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>208</v>
       </c>
@@ -18892,7 +18894,7 @@
         <v>3.942354411520081</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>209</v>
       </c>
@@ -18932,7 +18934,7 @@
         <v>15.151361866666635</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>210</v>
       </c>
@@ -18972,7 +18974,7 @@
         <v>7.1358949311999771</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>211</v>
       </c>
@@ -19012,7 +19014,7 @@
         <v>5.6753237333318565E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>212</v>
       </c>
@@ -19052,7 +19054,7 @@
         <v>0.14758329599999834</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>213</v>
       </c>
@@ -19092,7 +19094,7 @@
         <v>0.82335322496000585</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>214</v>
       </c>
@@ -19132,7 +19134,7 @@
         <v>6.7899292159998417E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>215</v>
       </c>
@@ -19172,7 +19174,7 @@
         <v>8.3382184106665619E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>216</v>
       </c>
@@ -19238,21 +19240,21 @@
         <v>1.930254666666667E-2</v>
       </c>
       <c r="I202">
-        <v>0.13893360524605511</v>
+        <v>0.108933605246055</v>
       </c>
       <c r="J202">
         <v>16.402428571428569</v>
       </c>
       <c r="K202" s="3">
         <f t="shared" si="6"/>
-        <v>1.4094631867675922</v>
+        <v>1.1051171250056302</v>
       </c>
       <c r="L202" s="3">
         <f t="shared" si="7"/>
-        <v>29.661065309866665</v>
-      </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+        <v>18.234585199948746</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>219</v>
       </c>
@@ -19292,7 +19294,7 @@
         <v>2.9963911443199183</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>220</v>
       </c>
@@ -19332,7 +19334,7 @@
         <v>22.429675080960013</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>221</v>
       </c>
@@ -19372,7 +19374,7 @@
         <v>0.94892129920000279</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>222</v>
       </c>
@@ -19412,7 +19414,7 @@
         <v>0.81909570773338858</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>223</v>
       </c>
@@ -19452,7 +19454,7 @@
         <v>0.31658340224000026</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>224</v>
       </c>
@@ -19492,7 +19494,7 @@
         <v>1.1165750161066648</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>225</v>
       </c>
@@ -19532,7 +19534,7 @@
         <v>1.7002940625066572</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>226</v>
       </c>
@@ -19572,7 +19574,7 @@
         <v>0.85762968753777247</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>227</v>
       </c>
@@ -19652,7 +19654,7 @@
         <v>19.352671729066827</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>229</v>
       </c>
@@ -19692,7 +19694,7 @@
         <v>0.94903962048000579</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>230</v>
       </c>
@@ -19732,7 +19734,7 @@
         <v>22.429675080959928</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>231</v>
       </c>
@@ -19772,7 +19774,7 @@
         <v>1.3346384277333756</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>232</v>
       </c>
@@ -19812,7 +19814,7 @@
         <v>1.6169755391998979</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>233</v>
       </c>
@@ -19852,7 +19854,7 @@
         <v>0.29834743679999898</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>234</v>
       </c>
@@ -19892,7 +19894,7 @@
         <v>1.6179863556266645</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>235</v>
       </c>
@@ -19932,7 +19934,7 @@
         <v>1.9061502596266702</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>236</v>
       </c>
@@ -19972,7 +19974,7 @@
         <v>0.69357168384000134</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>237</v>
       </c>
@@ -20012,7 +20014,7 @@
         <v>14.838224656418049</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>238</v>
       </c>
@@ -20043,16 +20045,16 @@
       <c r="J222">
         <v>9.9765714285714289</v>
       </c>
-      <c r="K222">
+      <c r="K222" s="3">
         <f t="shared" si="6"/>
         <v>1.6281204948894037</v>
       </c>
-      <c r="L222">
+      <c r="L222" s="3">
         <f t="shared" si="7"/>
         <v>14.641922534399894</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>239</v>
       </c>
@@ -20092,7 +20094,7 @@
         <v>28.323110300799904</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>240</v>
       </c>
@@ -20132,7 +20134,7 @@
         <v>13.333198442666687</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>241</v>
       </c>
@@ -20172,7 +20174,7 @@
         <v>0.88598052479999234</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>242</v>
       </c>
@@ -20212,7 +20214,7 @@
         <v>1.2688702357333195</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>243</v>
       </c>
@@ -20252,7 +20254,7 @@
         <v>0.17777051562666921</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>244</v>
       </c>
@@ -20292,7 +20294,7 @@
         <v>0.21748607402666367</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>245</v>
       </c>
@@ -20332,7 +20334,7 @@
         <v>1.2188726532266663</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>246</v>
       </c>
@@ -20372,7 +20374,7 @@
         <v>7.208907527111201E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>247</v>
       </c>
@@ -20452,7 +20454,7 @@
         <v>18.883292601600075</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>249</v>
       </c>
@@ -20492,7 +20494,7 @@
         <v>8.0684663807998636</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>250</v>
       </c>
@@ -20532,7 +20534,7 @@
         <v>10.908980544000039</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>251</v>
       </c>
@@ -20572,7 +20574,7 @@
         <v>0.65968467413340082</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>252</v>
       </c>
@@ -20612,7 +20614,7 @@
         <v>4.6131930432000043</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>253</v>
       </c>
@@ -20652,7 +20654,7 @@
         <v>7.4845343999998953E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>254</v>
       </c>
@@ -20692,7 +20694,7 @@
         <v>0.28724806655999857</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>255</v>
       </c>
@@ -20732,7 +20734,7 @@
         <v>0.35061924650666526</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>256</v>
       </c>
@@ -20772,7 +20774,7 @@
         <v>0.177256716871111</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>257</v>
       </c>
@@ -20813,7 +20815,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L241" xr:uid="{7B62AD6E-4C46-4D86-966D-E6532A5E9179}"/>
+  <autoFilter ref="A1:L241" xr:uid="{7B62AD6E-4C46-4D86-966D-E6532A5E9179}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1185"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20822,8 +20830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB0B1FC-BAB3-441C-BF67-17CEED47D5B3}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20860,12 +20868,6 @@
       <c r="C3">
         <v>17</v>
       </c>
-      <c r="E3">
-        <v>1700</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
       <c r="G3">
         <v>8</v>
       </c>
@@ -20913,12 +20915,6 @@
       <c r="C8">
         <v>17</v>
       </c>
-      <c r="E8">
-        <v>2050</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
       <c r="G8">
         <v>5</v>
       </c>
@@ -20967,19 +20963,13 @@
         <v>7</v>
       </c>
       <c r="G13">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="E14">
-        <v>1185</v>
-      </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
       <c r="G14">
         <v>18</v>
       </c>
@@ -20988,12 +20978,6 @@
       <c r="C15">
         <v>17</v>
       </c>
-      <c r="E15">
-        <v>1185</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
       <c r="G15">
         <v>19</v>
       </c>
@@ -21002,26 +20986,14 @@
       <c r="C16">
         <v>17</v>
       </c>
-      <c r="E16">
-        <v>1185</v>
-      </c>
-      <c r="F16">
-        <v>7</v>
-      </c>
       <c r="G16">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>17</v>
       </c>
-      <c r="E17">
-        <v>1185</v>
-      </c>
-      <c r="F17">
-        <v>7</v>
-      </c>
       <c r="G17">
         <v>20</v>
       </c>
@@ -21038,55 +21010,54 @@
       <c r="C19">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
-        <v>265</v>
-      </c>
-      <c r="G19" s="4">
-        <f>AVERAGE(G13:G18)</f>
-        <v>24</v>
+      <c r="G19">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>16</v>
       </c>
+      <c r="G20">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>17</v>
       </c>
+      <c r="F21" t="s">
+        <v>265</v>
+      </c>
+      <c r="G21" s="5">
+        <f>AVERAGE(G13:G20)</f>
+        <v>17.75</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>17</v>
       </c>
-      <c r="G22" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>17</v>
       </c>
-      <c r="E23">
-        <v>915</v>
-      </c>
-      <c r="F23">
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>15</v>
+      <c r="G23" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>30</v>
       </c>
-      <c r="F24" t="s">
-        <v>265</v>
-      </c>
-      <c r="G24" s="4">
-        <f>AVERAGE(G23)</f>
+      <c r="E24">
+        <v>915</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
         <v>15</v>
       </c>
     </row>
@@ -21094,44 +21065,51 @@
       <c r="C25">
         <v>36</v>
       </c>
+      <c r="F25" t="s">
+        <v>265</v>
+      </c>
+      <c r="G25" s="4">
+        <f>AVERAGE(G24)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>25</v>
       </c>
-      <c r="G26" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>17</v>
       </c>
-      <c r="E27">
-        <v>1470</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-      <c r="G27">
-        <v>9</v>
+      <c r="G27" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>16</v>
       </c>
-      <c r="F28" t="s">
-        <v>265</v>
-      </c>
-      <c r="G28" s="4">
-        <f>AVERAGE(G27)</f>
+      <c r="E28">
+        <v>1470</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>265</v>
+      </c>
+      <c r="G29" s="4">
+        <f>AVERAGE(G28)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>